<commit_message>
excel funcitonality almost done
</commit_message>
<xml_diff>
--- a/ganttproject-builder/dist-bin/test.xlsx
+++ b/ganttproject-builder/dist-bin/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dany5\Desktop\ApachePOITest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dany5\Desktop\ganttproject\ganttproject-builder\dist-bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCC0DAB-724C-4974-99E1-9043024F2AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CCB57F-DB01-4558-90DD-959D3A5C5724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D1348EB-CC72-4B03-A05F-A6AB50F8B075}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Daniel</t>
   </si>
   <si>
-    <t>Inginheiro</t>
-  </si>
-  <si>
     <t>Armando</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>jogadorDaBola</t>
+  </si>
+  <si>
+    <t>programador</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,40 +427,40 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>300</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel PROBABLY fully functional/need to look for bugs
</commit_message>
<xml_diff>
--- a/ganttproject-builder/dist-bin/test.xlsx
+++ b/ganttproject-builder/dist-bin/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dany5\Desktop\ganttproject\ganttproject-builder\dist-bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CCB57F-DB01-4558-90DD-959D3A5C5724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9195DF29-D7CE-4582-B80C-332164B6DCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D1348EB-CC72-4B03-A05F-A6AB50F8B075}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Daniel</t>
   </si>
@@ -60,16 +60,39 @@
   </si>
   <si>
     <t>programador</t>
+  </si>
+  <si>
+    <t>d.eugenio@campus.fct.pt</t>
+  </si>
+  <si>
+    <t>armando@gmail.com</t>
+  </si>
+  <si>
+    <t>armindo@hotmail.com</t>
+  </si>
+  <si>
+    <t>carlitos@iol.pt</t>
+  </si>
+  <si>
+    <t>960157851</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,13 +115,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -411,59 +438,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEC3B70-0BBF-463D-ACFC-73F7BEB3DD07}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
+        <v>967653994</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
+        <v>919191223</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
+        <v>925566778</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
         <v>300</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{4E00CDED-BE5C-4CB4-93F1-8A010B9EC118}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{BBE5A7F5-B405-40E0-A46D-10D563FF4B73}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{394B989B-9AA8-408E-88CB-416B8E58204C}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{0045C494-978C-4F2A-B1A4-45EBB54AB24E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new excel file TESTING
</commit_message>
<xml_diff>
--- a/ganttproject-builder/dist-bin/test.xlsx
+++ b/ganttproject-builder/dist-bin/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dany5\Desktop\ganttproject\ganttproject-builder\dist-bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D761058A-84BB-4B77-AA57-B428B53DB577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B7C3A2-B0AD-4413-A143-0E1111A61674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D1348EB-CC72-4B03-A05F-A6AB50F8B075}"/>
   </bookViews>
@@ -447,7 +447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEC3B70-0BBF-463D-ACFC-73F7BEB3DD07}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>